<commit_message>
Add annual station capacity factor
Add annual station capacity factor as an input parameter. Update cost and emissions calculations to incorporate station capacity factor.
</commit_message>
<xml_diff>
--- a/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
+++ b/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/modeling/model - LOCAL COPY/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/analyses/hydrogen_networks/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F45A9C-F972-4F09-89A3-E15A77E02977}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5249FE22-BF66-4F20-A837-EA857A46B405}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
       <text>
         <r>
           <rPr>
@@ -185,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
       <text>
         <r>
           <rPr>
@@ -235,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
       <text>
         <r>
           <rPr>
@@ -260,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
       <text>
         <r>
           <rPr>
@@ -285,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
       <text>
         <r>
           <rPr>
@@ -310,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
       <text>
         <r>
           <rPr>
@@ -334,7 +334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
       <text>
         <r>
           <rPr>
@@ -430,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{214B6BAD-4E8B-4B8C-9A1B-A05799FF452B}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{214B6BAD-4E8B-4B8C-9A1B-A05799FF452B}">
       <text>
         <r>
           <rPr>
@@ -455,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{CD78496C-361F-4AA2-A7B5-C49F252EFCEA}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{CD78496C-361F-4AA2-A7B5-C49F252EFCEA}">
       <text>
         <r>
           <rPr>
@@ -480,7 +480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{6E182C7D-C4A7-4883-AEF9-502B2BDB4F6F}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{6E182C7D-C4A7-4883-AEF9-502B2BDB4F6F}">
       <text>
         <r>
           <rPr>
@@ -505,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{A4A58B15-9A8C-4A09-8F6B-3EA07859A592}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{A4A58B15-9A8C-4A09-8F6B-3EA07859A592}">
       <text>
         <r>
           <rPr>
@@ -530,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{ED41E46E-89DA-4353-BA76-6AC3E7C714C9}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{ED41E46E-89DA-4353-BA76-6AC3E7C714C9}">
       <text>
         <r>
           <rPr>
@@ -555,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
       <text>
         <r>
           <rPr>
@@ -585,7 +585,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>run #</t>
   </si>
@@ -714,6 +714,12 @@
   </si>
   <si>
     <t>closed loop</t>
+  </si>
+  <si>
+    <t>station annual capacity factor</t>
+  </si>
+  <si>
+    <t>closed loop 80 cap factor</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1310,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1607,57 +1609,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AM5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="43" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="43" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1671,109 +1674,112 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1787,48 +1793,48 @@
         <v>1000</v>
       </c>
       <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
         <v>10</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>100</v>
       </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G4" si="0">17.09/100</f>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H5" si="0">17.09/100</f>
         <v>0.1709</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>6.0279999999999996</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>0.22800000000000001</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>10.18</v>
       </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
       <c r="L2" s="1">
         <v>0</v>
       </c>
       <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <v>0.31</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>366.15</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>105</v>
       </c>
-      <c r="R2" s="1">
-        <v>1</v>
-      </c>
       <c r="S2" s="1">
         <v>1</v>
       </c>
@@ -1836,66 +1842,69 @@
         <v>1</v>
       </c>
       <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
         <v>53</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>5450</v>
       </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1">
         <v>0</v>
       </c>
       <c r="Z2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
         <v>5250</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AB2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AC2" s="1">
         <v>300</v>
       </c>
-      <c r="AC2" s="1">
-        <v>1</v>
-      </c>
       <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AF2" s="1">
-        <v>1</v>
-      </c>
       <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AI2" s="1">
         <v>3500</v>
       </c>
-      <c r="AI2" s="1">
-        <v>1</v>
-      </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK2" s="1">
         <v>0</v>
       </c>
       <c r="AL2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B4" si="1">B2+1</f>
+        <f t="shared" ref="B3:B5" si="1">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1905,27 +1914,27 @@
         <v>1000</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>100</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <f t="shared" si="0"/>
         <v>0.1709</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>6.0279999999999996</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>10.18</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
         <v>0</v>
       </c>
@@ -1935,18 +1944,18 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
         <v>38</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>366.15</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>105</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
       <c r="S3">
         <v>1</v>
       </c>
@@ -1954,61 +1963,64 @@
         <v>1</v>
       </c>
       <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
         <v>53</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>5450</v>
       </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
         <v>5250</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>0.25</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>300</v>
       </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
       <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
       <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>3500</v>
       </c>
-      <c r="AI3">
-        <v>1</v>
-      </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK3">
         <v>0</v>
       </c>
       <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2023,48 +2035,48 @@
         <v>1000</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>0.1709</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>6.0279999999999996</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>10.18</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>0.31</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
         <v>35</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>366.15</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>105</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
       <c r="S4">
         <v>1</v>
       </c>
@@ -2072,62 +2084,186 @@
         <v>1</v>
       </c>
       <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
         <v>53</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>5450</v>
       </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
         <v>5250</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>0.25</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>300</v>
       </c>
-      <c r="AC4">
-        <v>1</v>
-      </c>
       <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
       <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>3500</v>
       </c>
-      <c r="AI4">
-        <v>1</v>
-      </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4">
         <v>0</v>
       </c>
       <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>0.8</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.1709</v>
+      </c>
+      <c r="I5">
+        <v>6.0279999999999996</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>10.18</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.31</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5">
+        <v>366.15</v>
+      </c>
+      <c r="R5">
+        <v>105</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>53</v>
+      </c>
+      <c r="W5">
+        <v>5450</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>5250</v>
+      </c>
+      <c r="AB5">
+        <v>0.25</v>
+      </c>
+      <c r="AC5">
+        <v>300</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="AF5">
+        <v>7.31028611028611E-2</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>9.6467120334224301</v>
+      </c>
+      <c r="AI5">
+        <v>3500</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AL4">
+  <conditionalFormatting sqref="C3:AM5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update input to "calcs" function
Add hydrogenation electrolyzer voltage and current density  as user-supplied input parameters to "calcs" function. (These were fixed parameters.)
</commit_message>
<xml_diff>
--- a/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
+++ b/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/analyses/hydrogen_networks/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5249FE22-BF66-4F20-A837-EA857A46B405}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EEA108A-2110-4A91-95B2-1C30A23E003B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
       <text>
         <r>
           <rPr>
@@ -555,7 +555,59 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{C26BA404-EDC2-4E3C-8D61-9D1F07B5884C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cell voltage for hydrogen oxidation. Calculated assuming a cell voltage of 2.5 V for water oxidation [1,2] and a reversible potential for water oxidation relative to hydrogen oxidation of 1.23 V (i.e., 2.5 V − 1.23 V = 1.27 V) [3].
+[1] B. S. Crandall, T. Brix, R. S. Weber and F. Jiao, Energ Fuel, 2022, 37, 1441-1450.
+[2] M. Ramdin, A. R. T. Morrison, M. de Groen, R. van Haperen, R. de Kler, L. J. P. van den Broeke, J. P. M. Trusler, W. de Jong and T. J. H. Vlugt, Ind Eng Chem Res, 2019, 58, 1834-1847.
+[3] W. Q. Li, J. T. Feaster, S. A. Akhade, J. T. Davis, A. A. Wong, V. A. Beck, J. B. Varley, S. A. Hawks, M. Stadermann, C. Hahn, R. D. Aines, E. B. Duoss and S. E. Baker, ACS Sustain Chem Eng, 2021, 9, 14678-14689.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{CE68BB1E-799F-4775-B8CB-797AF6A59114}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[1] B. S. Crandall, T. Brix, R. S. Weber and F. Jiao, Energ Fuel, 2022, 37, 1441-1450.
+[2] M. Ramdin, A. R. T. Morrison, M. de Groen, R. van Haperen, R. de Kler, L. J. P. van den Broeke, J. P. M. Trusler, W. de Jong and T. J. H. Vlugt, Ind Eng Chem Res, 2019, 58, 1834-1847.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
       <text>
         <r>
           <rPr>
@@ -585,7 +637,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>run #</t>
   </si>
@@ -710,16 +762,22 @@
     <t>station formic acid storage amount (days)</t>
   </si>
   <si>
-    <t>delivery only</t>
-  </si>
-  <si>
-    <t>closed loop</t>
-  </si>
-  <si>
     <t>station annual capacity factor</t>
   </si>
   <si>
-    <t>closed loop 80 cap factor</t>
+    <t>FA - delivery only</t>
+  </si>
+  <si>
+    <t>FA - closed loop</t>
+  </si>
+  <si>
+    <t>FA - closed loop - 80 cap factor</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer voltage (V)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer current density (A/m^2)</t>
   </si>
 </sst>
 </file>
@@ -1609,18 +1667,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM5"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -1644,23 +1702,25 @@
     <col min="23" max="23" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="31" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="43" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="43" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1674,7 +1734,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -1737,49 +1797,55 @@
         <v>22</v>
       </c>
       <c r="Z1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1857,51 +1923,57 @@
         <v>0</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="AA2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
         <v>5250</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AD2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AE2" s="1">
         <v>300</v>
       </c>
-      <c r="AD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AH2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AG2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="1">
+      <c r="AI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AK2" s="1">
         <v>3500</v>
       </c>
-      <c r="AJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>0</v>
-      </c>
       <c r="AL2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B5" si="1">B2+1</f>
@@ -1978,51 +2050,57 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="AA3">
+        <v>2000</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
         <v>5250</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>0.25</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>300</v>
       </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
-      <c r="AE3">
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AF3">
+      <c r="AH3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AH3">
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>3500</v>
       </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
       <c r="AL3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
@@ -2099,49 +2177,55 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="AA4">
+        <v>2000</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
         <v>5250</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>0.25</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>300</v>
       </c>
-      <c r="AD4">
-        <v>1</v>
-      </c>
-      <c r="AE4">
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AG4">
-        <v>1</v>
-      </c>
-      <c r="AH4">
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>3500</v>
       </c>
-      <c r="AJ4">
-        <v>1</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
       <c r="AL4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2220,50 +2304,56 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="AA5">
+        <v>2000</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
         <v>5250</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>0.25</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>300</v>
       </c>
-      <c r="AD5">
-        <v>1</v>
-      </c>
-      <c r="AE5">
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AG5">
-        <v>1</v>
-      </c>
-      <c r="AH5">
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>3500</v>
       </c>
-      <c r="AJ5">
-        <v>1</v>
-      </c>
-      <c r="AK5">
-        <v>0</v>
-      </c>
       <c r="AL5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AM5">
+  <conditionalFormatting sqref="C3:AO5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>

</xml_diff>

<commit_message>
Generalize hydrogen carrier mass balance
Generalize mass balance for user-supplied hydrogen carrier. Hydrogen carriers are characterized by name, molar mass, density, and stoichiometry.
</commit_message>
<xml_diff>
--- a/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
+++ b/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/analyses/hydrogen_networks/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EEA108A-2110-4A91-95B2-1C30A23E003B}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0990156E-7DE8-4A3B-BAE8-EBB080CF406E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{ACA71E89-892C-48A7-882C-1D446A4F3744}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Use in delivery pathway name (in output files).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E91F5129-45DF-4C7E-98CB-9EB0ECA2B407}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+At target transport and storage conditions for given LOHC.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
       <text>
         <r>
           <rPr>
@@ -135,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
       <text>
         <r>
           <rPr>
@@ -160,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
       <text>
         <r>
           <rPr>
@@ -185,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
       <text>
         <r>
           <rPr>
@@ -210,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
       <text>
         <r>
           <rPr>
@@ -235,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
       <text>
         <r>
           <rPr>
@@ -260,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
       <text>
         <r>
           <rPr>
@@ -285,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
       <text>
         <r>
           <rPr>
@@ -310,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
       <text>
         <r>
           <rPr>
@@ -334,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
       <text>
         <r>
           <rPr>
@@ -358,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
       <text>
         <r>
           <rPr>
@@ -382,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
       <text>
         <r>
           <rPr>
@@ -555,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{C26BA404-EDC2-4E3C-8D61-9D1F07B5884C}">
+    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{C26BA404-EDC2-4E3C-8D61-9D1F07B5884C}">
       <text>
         <r>
           <rPr>
@@ -582,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{CE68BB1E-799F-4775-B8CB-797AF6A59114}">
+    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{CE68BB1E-799F-4775-B8CB-797AF6A59114}">
       <text>
         <r>
           <rPr>
@@ -607,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
+    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
       <text>
         <r>
           <rPr>
@@ -637,7 +685,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>run #</t>
   </si>
@@ -669,18 +717,9 @@
     <t>hydrogen prod. emission factor (kg CO2-eq/kg)</t>
   </si>
   <si>
-    <t>formic acid prod. emission factor (kg CO2-eq/kg)</t>
-  </si>
-  <si>
     <t>hydrogen purchase cost ($/kg)</t>
   </si>
   <si>
-    <t>formic acid purchase cost ($/kg)</t>
-  </si>
-  <si>
-    <t>formic acid production pathway</t>
-  </si>
-  <si>
     <t>hydr. reaction temperature (K)</t>
   </si>
   <si>
@@ -756,12 +795,6 @@
     <t>purchase</t>
   </si>
   <si>
-    <t>terminal formic acid storage amount (days)</t>
-  </si>
-  <si>
-    <t>station formic acid storage amount (days)</t>
-  </si>
-  <si>
     <t>station annual capacity factor</t>
   </si>
   <si>
@@ -778,6 +811,42 @@
   </si>
   <si>
     <t>hydr. electrolyzer current density (A/m^2)</t>
+  </si>
+  <si>
+    <t>LOHC prod. emission factor (kg CO2-eq/kg)</t>
+  </si>
+  <si>
+    <t>LOHC purchase cost ($/kg)</t>
+  </si>
+  <si>
+    <t>LOHC production pathway</t>
+  </si>
+  <si>
+    <t>terminal LOHC storage amount (days)</t>
+  </si>
+  <si>
+    <t>station LOHC storage amount (days)</t>
+  </si>
+  <si>
+    <t>LOHC name</t>
+  </si>
+  <si>
+    <t>formic acid</t>
+  </si>
+  <si>
+    <t>LOHC molar mass (kg/kmol)</t>
+  </si>
+  <si>
+    <t>LOHC density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>stoic. ratio (mol e/mol LOHC)</t>
+  </si>
+  <si>
+    <t>stoic. ratio (mol H2/mol LOHC)</t>
+  </si>
+  <si>
+    <t>stoic. ratio (mol CO2/mol LOHC)</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1415,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1667,22 +1746,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO5"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AR3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA1" sqref="AA1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
@@ -1690,39 +1769,46 @@
     <col min="10" max="10" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="31" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="43" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="43" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1734,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -1758,96 +1844,114 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -1893,87 +1997,105 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="1">
+        <v>46.024999999999999</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1220</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="1">
         <v>366.15</v>
       </c>
-      <c r="R2" s="1">
+      <c r="X2" s="1">
         <v>105</v>
       </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1">
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
         <v>53</v>
       </c>
-      <c r="W2" s="1">
+      <c r="AC2" s="1">
         <v>5450</v>
       </c>
-      <c r="X2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1">
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
         <v>1.27</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AG2" s="1">
         <v>2000</v>
       </c>
-      <c r="AB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1">
+      <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
         <v>5250</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AJ2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AK2" s="1">
         <v>300</v>
       </c>
-      <c r="AF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="1">
+      <c r="AL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AN2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="1">
+      <c r="AO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AQ2" s="1">
         <v>3500</v>
       </c>
-      <c r="AL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="1">
+      <c r="AR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B5" si="1">B2+1</f>
@@ -2020,87 +2142,105 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3">
+        <v>46.024999999999999</v>
+      </c>
+      <c r="R3">
+        <v>1220</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3">
+        <v>366.15</v>
+      </c>
+      <c r="X3">
+        <v>105</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>53</v>
+      </c>
+      <c r="AC3">
+        <v>5450</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>1.27</v>
+      </c>
+      <c r="AG3">
+        <v>2000</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>5250</v>
+      </c>
+      <c r="AJ3">
+        <v>0.25</v>
+      </c>
+      <c r="AK3">
+        <v>300</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="AN3">
+        <v>7.31028611028611E-2</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>9.6467120334224301</v>
+      </c>
+      <c r="AQ3">
+        <v>3500</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>38</v>
-      </c>
-      <c r="Q3">
-        <v>366.15</v>
-      </c>
-      <c r="R3">
-        <v>105</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>53</v>
-      </c>
-      <c r="W3">
-        <v>5450</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>1.27</v>
-      </c>
-      <c r="AA3">
-        <v>2000</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>5250</v>
-      </c>
-      <c r="AD3">
-        <v>0.25</v>
-      </c>
-      <c r="AE3">
-        <v>300</v>
-      </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="AH3">
-        <v>7.31028611028611E-2</v>
-      </c>
-      <c r="AI3">
-        <v>1</v>
-      </c>
-      <c r="AJ3">
-        <v>9.6467120334224301</v>
-      </c>
-      <c r="AK3">
-        <v>3500</v>
-      </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
@@ -2147,87 +2287,105 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q4">
+        <v>46.024999999999999</v>
+      </c>
+      <c r="R4">
+        <v>1220</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W4">
         <v>366.15</v>
       </c>
-      <c r="R4">
+      <c r="X4">
         <v>105</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>1</v>
-      </c>
-      <c r="V4">
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
         <v>53</v>
       </c>
-      <c r="W4">
+      <c r="AC4">
         <v>5450</v>
       </c>
-      <c r="X4">
-        <v>1</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
         <v>1.27</v>
       </c>
-      <c r="AA4">
+      <c r="AG4">
         <v>2000</v>
       </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
         <v>5250</v>
       </c>
-      <c r="AD4">
+      <c r="AJ4">
         <v>0.25</v>
       </c>
-      <c r="AE4">
+      <c r="AK4">
         <v>300</v>
       </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
-      <c r="AG4">
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AH4">
+      <c r="AN4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AI4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
+      <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AP4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AK4">
+      <c r="AQ4">
         <v>3500</v>
       </c>
-      <c r="AL4">
-        <v>1</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
+      <c r="AR4">
+        <v>1</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
@@ -2274,86 +2432,104 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q5">
+        <v>46.024999999999999</v>
+      </c>
+      <c r="R5">
+        <v>1220</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5">
         <v>366.15</v>
       </c>
-      <c r="R5">
+      <c r="X5">
         <v>105</v>
       </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
-      <c r="V5">
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
         <v>53</v>
       </c>
-      <c r="W5">
+      <c r="AC5">
         <v>5450</v>
       </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
         <v>1.27</v>
       </c>
-      <c r="AA5">
+      <c r="AG5">
         <v>2000</v>
       </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <v>5250</v>
       </c>
-      <c r="AD5">
+      <c r="AJ5">
         <v>0.25</v>
       </c>
-      <c r="AE5">
+      <c r="AK5">
         <v>300</v>
       </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-      <c r="AG5">
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AH5">
+      <c r="AN5">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AI5">
-        <v>1</v>
-      </c>
-      <c r="AJ5">
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AK5">
+      <c r="AQ5">
         <v>3500</v>
       </c>
-      <c r="AL5">
-        <v>1</v>
-      </c>
-      <c r="AM5">
-        <v>0</v>
-      </c>
-      <c r="AN5">
-        <v>0</v>
-      </c>
-      <c r="AO5">
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AO5">
+  <conditionalFormatting sqref="C3:AU5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update electrolyzer power and cost calculations
Incorporate electrolyzer model outputs as inputs to electrolyzer power and cost (installed and O&M costs) calculations.
</commit_message>
<xml_diff>
--- a/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
+++ b/analyses/hydrogen_networks/inputs/input params_baseline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/analyses/hydrogen_networks/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0990156E-7DE8-4A3B-BAE8-EBB080CF406E}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2781DDC-0380-44D4-95C3-8F39AEE8F723}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
       <text>
         <r>
           <rPr>
@@ -183,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
       <text>
         <r>
           <rPr>
@@ -208,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
       <text>
         <r>
           <rPr>
@@ -233,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
       <text>
         <r>
           <rPr>
@@ -258,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
       <text>
         <r>
           <rPr>
@@ -283,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
       <text>
         <r>
           <rPr>
@@ -308,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
       <text>
         <r>
           <rPr>
@@ -333,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
       <text>
         <r>
           <rPr>
@@ -406,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
       <text>
         <r>
           <rPr>
@@ -430,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
       <text>
         <r>
           <rPr>
@@ -603,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{C26BA404-EDC2-4E3C-8D61-9D1F07B5884C}">
+    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{C26BA404-EDC2-4E3C-8D61-9D1F07B5884C}">
       <text>
         <r>
           <rPr>
@@ -630,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{CE68BB1E-799F-4775-B8CB-797AF6A59114}">
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{CE68BB1E-799F-4775-B8CB-797AF6A59114}">
       <text>
         <r>
           <rPr>
@@ -655,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
+    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
       <text>
         <r>
           <rPr>
@@ -685,7 +685,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>run #</t>
   </si>
@@ -840,13 +840,16 @@
     <t>LOHC density (kg/m^3)</t>
   </si>
   <si>
-    <t>stoic. ratio (mol e/mol LOHC)</t>
-  </si>
-  <si>
     <t>stoic. ratio (mol H2/mol LOHC)</t>
   </si>
   <si>
     <t>stoic. ratio (mol CO2/mol LOHC)</t>
+  </si>
+  <si>
+    <t>hydr. LOHC output flowrate (kg/s)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer cell area (m^2/cell)</t>
   </si>
 </sst>
 </file>
@@ -1365,11 +1368,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1415,17 +1419,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1746,13 +1740,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU5"/>
+  <dimension ref="A1:AV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="AR3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,36 +1771,37 @@
     <col min="18" max="18" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="31" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="43" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.85546875" customWidth="1"/>
+    <col min="32" max="32" width="34.140625" customWidth="1"/>
+    <col min="33" max="33" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="31" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="43" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1861,95 +1856,98 @@
       <c r="R1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -2011,17 +2009,17 @@
       <c r="T2" s="1">
         <v>1</v>
       </c>
-      <c r="U2" s="1">
-        <v>2</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="V2" s="1">
+        <v>366.15</v>
+      </c>
       <c r="W2" s="1">
-        <v>366.15</v>
+        <v>105</v>
       </c>
       <c r="X2" s="1">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1">
         <v>1</v>
@@ -2030,75 +2028,80 @@
         <v>1</v>
       </c>
       <c r="AA2" s="1">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="AB2" s="1">
-        <v>53</v>
+        <v>5450</v>
       </c>
       <c r="AC2" s="1">
-        <v>5450</v>
+        <v>1</v>
       </c>
       <c r="AD2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <v>0</v>
+        <f t="shared" ref="AE2:AE5" si="1">D2/2.016/S2*Q2/AN2/24/3600*F2</f>
+        <v>2.6426092969379242</v>
       </c>
       <c r="AF2" s="1">
+        <f t="shared" ref="AF2:AF5" si="2">2*96485/AH2*AE2</f>
+        <v>254.97215801505561</v>
+      </c>
+      <c r="AG2" s="1">
         <v>1.27</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AH2" s="1">
         <v>2000</v>
       </c>
-      <c r="AH2" s="1">
-        <v>0</v>
-      </c>
       <c r="AI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
         <v>5250</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AK2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AL2" s="1">
         <v>300</v>
       </c>
-      <c r="AL2" s="1">
-        <v>1</v>
-      </c>
       <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AO2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AO2" s="1">
-        <v>1</v>
-      </c>
       <c r="AP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AQ2" s="1">
+      <c r="AR2" s="1">
         <v>3500</v>
       </c>
-      <c r="AR2" s="1">
-        <v>1</v>
-      </c>
       <c r="AS2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT2" s="1">
         <v>0</v>
       </c>
       <c r="AU2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B5" si="1">B2+1</f>
+        <f t="shared" ref="B3:B5" si="3">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -2156,17 +2159,17 @@
       <c r="T3">
         <v>1</v>
       </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="U3" t="s">
         <v>35</v>
       </c>
+      <c r="V3">
+        <v>366.15</v>
+      </c>
       <c r="W3">
-        <v>366.15</v>
+        <v>105</v>
       </c>
       <c r="X3">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="Y3">
         <v>1</v>
@@ -2175,75 +2178,80 @@
         <v>1</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="AB3">
-        <v>53</v>
+        <v>5450</v>
       </c>
       <c r="AC3">
-        <v>5450</v>
+        <v>1</v>
       </c>
       <c r="AD3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.6426092969379242</v>
       </c>
       <c r="AF3">
+        <f t="shared" si="2"/>
+        <v>254.97215801505561</v>
+      </c>
+      <c r="AG3">
         <v>1.27</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>2000</v>
       </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
       <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
         <v>5250</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>0.25</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>300</v>
       </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
       <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
       <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>3500</v>
       </c>
-      <c r="AR3">
-        <v>1</v>
-      </c>
       <c r="AS3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT3">
         <v>0</v>
       </c>
       <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="C4">
@@ -2301,17 +2309,17 @@
       <c r="T4">
         <v>1</v>
       </c>
-      <c r="U4">
-        <v>2</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="U4" t="s">
         <v>32</v>
       </c>
+      <c r="V4">
+        <v>366.15</v>
+      </c>
       <c r="W4">
-        <v>366.15</v>
+        <v>105</v>
       </c>
       <c r="X4">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="Y4">
         <v>1</v>
@@ -2320,75 +2328,80 @@
         <v>1</v>
       </c>
       <c r="AA4">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="AB4">
-        <v>53</v>
+        <v>5450</v>
       </c>
       <c r="AC4">
-        <v>5450</v>
+        <v>1</v>
       </c>
       <c r="AD4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.6426092969379242</v>
       </c>
       <c r="AF4">
+        <f t="shared" si="2"/>
+        <v>254.97215801505561</v>
+      </c>
+      <c r="AG4">
         <v>1.27</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>2000</v>
       </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
       <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
         <v>5250</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>0.25</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>300</v>
       </c>
-      <c r="AL4">
-        <v>1</v>
-      </c>
       <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AO4">
-        <v>1</v>
-      </c>
       <c r="AP4">
+        <v>1</v>
+      </c>
+      <c r="AQ4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>3500</v>
       </c>
-      <c r="AR4">
-        <v>1</v>
-      </c>
       <c r="AS4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT4">
         <v>0</v>
       </c>
       <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="C5">
@@ -2446,17 +2459,17 @@
       <c r="T5">
         <v>1</v>
       </c>
-      <c r="U5">
-        <v>2</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="U5" t="s">
         <v>32</v>
       </c>
+      <c r="V5">
+        <v>366.15</v>
+      </c>
       <c r="W5">
-        <v>366.15</v>
+        <v>105</v>
       </c>
       <c r="X5">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="Y5">
         <v>1</v>
@@ -2465,71 +2478,76 @@
         <v>1</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="AB5">
-        <v>53</v>
+        <v>5450</v>
       </c>
       <c r="AC5">
-        <v>5450</v>
+        <v>1</v>
       </c>
       <c r="AD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.6426092969379242</v>
       </c>
       <c r="AF5">
+        <f t="shared" si="2"/>
+        <v>254.97215801505561</v>
+      </c>
+      <c r="AG5">
         <v>1.27</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>2000</v>
       </c>
-      <c r="AH5">
-        <v>0</v>
-      </c>
       <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
         <v>5250</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>0.25</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>300</v>
       </c>
-      <c r="AL5">
-        <v>1</v>
-      </c>
       <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
       <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>3500</v>
       </c>
-      <c r="AR5">
-        <v>1</v>
-      </c>
       <c r="AS5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT5">
         <v>0</v>
       </c>
       <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AU5">
+  <conditionalFormatting sqref="C3:AV5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>
@@ -2537,4 +2555,297 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001B4E99C690CD84D8C14FB9B89CF5CA2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d6ebaee038f40569f500d908425f89c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="72d00a49-d4df-4ae2-8448-0e7c38748169" xmlns:ns3="cdbd341c-9425-4527-8200-dbc5093c0c26" xmlns:ns4="cc3aaed6-9815-470c-8f7f-f66d9ca72b53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d22da384523c48d606acb8860bdc860" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
+    <xsd:import namespace="cdbd341c-9425-4527-8200-dbc5093c0c26"/>
+    <xsd:import namespace="cc3aaed6-9815-470c-8f7f-f66d9ca72b53"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="72d00a49-d4df-4ae2-8448-0e7c38748169" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="93a22c89-3912-4715-9657-2989270db28b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="17" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="20" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="21" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cdbd341c-9425-4527-8200-dbc5093c0c26" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{453f2cc4-5f9f-4bbb-9939-0cc4669e82ba}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="cc3aaed6-9815-470c-8f7f-f66d9ca72b53">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cc3aaed6-9815-470c-8f7f-f66d9ca72b53" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="72d00a49-d4df-4ae2-8448-0e7c38748169">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cdbd341c-9425-4527-8200-dbc5093c0c26" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2DAFF9-D831-4A8A-A26B-34A3990B404D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
+    <ds:schemaRef ds:uri="cdbd341c-9425-4527-8200-dbc5093c0c26"/>
+    <ds:schemaRef ds:uri="cc3aaed6-9815-470c-8f7f-f66d9ca72b53"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
+    <ds:schemaRef ds:uri="cdbd341c-9425-4527-8200-dbc5093c0c26"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>